<commit_message>
fix ekyc and file import
</commit_message>
<xml_diff>
--- a/src/assets/upload/import_nguoi_dung.xlsx
+++ b/src/assets/upload/import_nguoi_dung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP Probook 440G8\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\econtract-web\src\assets\upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B473DD33-4AFA-4773-BF71-D2C3223EDC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C3F154-5C99-443C-93AE-0D42F500BDD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,10 +87,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -375,7 +376,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,7 +384,7 @@
     <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="3" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" customWidth="1"/>
     <col min="6" max="6" width="13.140625" customWidth="1"/>
   </cols>
@@ -398,7 +399,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">

</xml_diff>